<commit_message>
EOD options close catch remaining only
</commit_message>
<xml_diff>
--- a/Rahul/BankniftyNifty/formula file.xlsx
+++ b/Rahul/BankniftyNifty/formula file.xlsx
@@ -435,8 +435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P164"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:I34"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,14 +444,16 @@
     <col min="1" max="1" width="33.42578125" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
     <col min="3" max="3" width="43.42578125" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" customWidth="1"/>
-    <col min="7" max="8" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" customWidth="1"/>
     <col min="11" max="11" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F1">
@@ -508,7 +510,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F5" t="s">
@@ -553,13 +555,13 @@
       <c r="C10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G10" t="s">

</xml_diff>